<commit_message>
Formatting update to XLSX file
</commit_message>
<xml_diff>
--- a/conf/resources/claim-vat-refund-diy-invoice-template.xlsx
+++ b/conf/resources/claim-vat-refund-diy-invoice-template.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominic.warren/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435AA5D2-F442-F142-87E7-2FA198C7D131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -37,18 +46,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -57,44 +68,54 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -284,28 +305,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.38"/>
-    <col customWidth="1" min="2" max="2" width="20.88"/>
-    <col customWidth="1" min="3" max="3" width="50.13"/>
-    <col customWidth="1" min="4" max="4" width="19.0"/>
-    <col customWidth="1" min="5" max="5" width="20.25"/>
-    <col customWidth="1" min="6" max="6" width="13.25"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -327,27 +353,27 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changing the spreadsheets to include 2 new columns
</commit_message>
<xml_diff>
--- a/conf/resources/claim-vat-refund-diy-invoice-template.xlsx
+++ b/conf/resources/claim-vat-refund-diy-invoice-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominic.warren/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominic.warren/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435AA5D2-F442-F142-87E7-2FA198C7D131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D095117D-F26C-B549-99E0-E1CC2BA4DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Invoice or receipt number</t>
   </si>
@@ -37,10 +37,13 @@
     <t>VAT registration number</t>
   </si>
   <si>
+    <t>Total invoice amount (excluding VAT)</t>
+  </si>
+  <si>
+    <t>Is the Invoice in your name? Y/N</t>
+  </si>
+  <si>
     <t>VAT amount</t>
-  </si>
-  <si>
-    <t>Total invoice amount (excluding VAT)</t>
   </si>
 </sst>
 </file>
@@ -71,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -80,21 +83,59 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -318,62 +359,69 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000OFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>